<commit_message>
Updated data simulation code, dashboard, and data.
</commit_message>
<xml_diff>
--- a/data/Benchmark_Data.xlsx
+++ b/data/Benchmark_Data.xlsx
@@ -436,14 +436,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Index_Benchmark</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Role_Benchmark</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Overall_Benchmark</t>
-        </is>
-      </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Work_Life_Balance_Benchmark</t>
@@ -471,353 +471,353 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>Accountant</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>74.9766081871345</v>
-      </c>
       <c r="C2" t="n">
-        <v>69.95614035087719</v>
+        <v>42.66457320065805</v>
       </c>
       <c r="D2" t="n">
-        <v>60.23684210526316</v>
+        <v>83.44394711474659</v>
       </c>
       <c r="E2" t="n">
-        <v>74.57309941520468</v>
+        <v>110.3736731718898</v>
       </c>
       <c r="F2" t="n">
-        <v>66.02046783625731</v>
+        <v>26.83152524691578</v>
       </c>
       <c r="G2" t="n">
-        <v>80.04385964912281</v>
+        <v>104.8291539435402</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Business Analyst</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>75.59556786703601</v>
-      </c>
       <c r="C3" t="n">
-        <v>71.73130193905817</v>
+        <v>32.07033993460573</v>
       </c>
       <c r="D3" t="n">
-        <v>58.48476454293629</v>
+        <v>51.42882730440155</v>
       </c>
       <c r="E3" t="n">
-        <v>74.25761772853186</v>
+        <v>27.10409715298731</v>
       </c>
       <c r="F3" t="n">
-        <v>65.77008310249307</v>
+        <v>41.3234115956139</v>
       </c>
       <c r="G3" t="n">
-        <v>79.78116343490305</v>
+        <v>81.89001172060458</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>Customer Support</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>74.95058139534883</v>
-      </c>
       <c r="C4" t="n">
-        <v>70.25290697674419</v>
+        <v>85.90819579932058</v>
       </c>
       <c r="D4" t="n">
-        <v>60.86918604651163</v>
+        <v>91.30494565446023</v>
       </c>
       <c r="E4" t="n">
-        <v>75.91860465116279</v>
+        <v>114.3055978810442</v>
       </c>
       <c r="F4" t="n">
-        <v>66.37209302325581</v>
+        <v>75.29002474858609</v>
       </c>
       <c r="G4" t="n">
-        <v>80.09011627906976</v>
+        <v>91.59631169145987</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>Data Analyst</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>74.48626373626374</v>
-      </c>
       <c r="C5" t="n">
-        <v>69.91483516483517</v>
+        <v>85.24068197080739</v>
       </c>
       <c r="D5" t="n">
-        <v>61.15384615384615</v>
+        <v>53.85237101017578</v>
       </c>
       <c r="E5" t="n">
-        <v>74.33241758241758</v>
+        <v>88.08546543371043</v>
       </c>
       <c r="F5" t="n">
-        <v>66.54945054945055</v>
+        <v>39.26178870883071</v>
       </c>
       <c r="G5" t="n">
-        <v>81.48626373626374</v>
+        <v>57.43328769992886</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Data Scientist</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>75.50139275766017</v>
-      </c>
       <c r="C6" t="n">
-        <v>70.83008356545962</v>
+        <v>58.29060015310971</v>
       </c>
       <c r="D6" t="n">
-        <v>61.15598885793872</v>
+        <v>24.26173277504419</v>
       </c>
       <c r="E6" t="n">
-        <v>74.84958217270194</v>
+        <v>62.93630877370196</v>
       </c>
       <c r="F6" t="n">
-        <v>63.45682451253482</v>
+        <v>104.9947959832414</v>
       </c>
       <c r="G6" t="n">
-        <v>80.16713091922006</v>
+        <v>80.61764733720652</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>HR Specialist</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>75.0828729281768</v>
-      </c>
       <c r="C7" t="n">
-        <v>70.73480662983425</v>
+        <v>98.02336050081948</v>
       </c>
       <c r="D7" t="n">
-        <v>59.89502762430939</v>
+        <v>104.2198591589407</v>
       </c>
       <c r="E7" t="n">
-        <v>74.90055248618785</v>
+        <v>47.63064210578121</v>
       </c>
       <c r="F7" t="n">
-        <v>66.51657458563535</v>
+        <v>38.5117707495847</v>
       </c>
       <c r="G7" t="n">
-        <v>79.75966850828729</v>
+        <v>123.9754787741175</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>Legal Advisor</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>75.22093023255815</v>
-      </c>
       <c r="C8" t="n">
-        <v>68.64244186046511</v>
+        <v>41.49928456059973</v>
       </c>
       <c r="D8" t="n">
-        <v>58.7296511627907</v>
+        <v>39.41613945827162</v>
       </c>
       <c r="E8" t="n">
-        <v>74.78197674418605</v>
+        <v>117.4910927359335</v>
       </c>
       <c r="F8" t="n">
-        <v>66.90697674418605</v>
+        <v>101.4742991576342</v>
       </c>
       <c r="G8" t="n">
-        <v>79.54360465116279</v>
+        <v>68.95778873870678</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>Machine Learning Engineer</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>74.92140921409214</v>
-      </c>
       <c r="C9" t="n">
-        <v>69.08943089430895</v>
+        <v>55.33196789161902</v>
       </c>
       <c r="D9" t="n">
-        <v>57.64769647696477</v>
+        <v>108.0914655182148</v>
       </c>
       <c r="E9" t="n">
-        <v>75.56639566395664</v>
+        <v>121.3040254051418</v>
       </c>
       <c r="F9" t="n">
-        <v>65.10840108401084</v>
+        <v>106.6021677754157</v>
       </c>
       <c r="G9" t="n">
-        <v>80.08401084010841</v>
+        <v>33.11104989979082</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>Marketing Manager</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>75.03977272727273</v>
-      </c>
       <c r="C10" t="n">
-        <v>70.79829545454545</v>
+        <v>76.93306421135722</v>
       </c>
       <c r="D10" t="n">
-        <v>61.32102272727273</v>
+        <v>11.83680526988351</v>
       </c>
       <c r="E10" t="n">
-        <v>73.46022727272727</v>
+        <v>46.35271529981099</v>
       </c>
       <c r="F10" t="n">
-        <v>64.40909090909091</v>
+        <v>69.34155507426746</v>
       </c>
       <c r="G10" t="n">
-        <v>80.10227272727273</v>
+        <v>59.86941548676152</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>Operations Manager</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>73.70810810810811</v>
-      </c>
       <c r="C11" t="n">
-        <v>69.71351351351352</v>
+        <v>117.8684676525102</v>
       </c>
       <c r="D11" t="n">
-        <v>58.81351351351351</v>
+        <v>34.93540751392739</v>
       </c>
       <c r="E11" t="n">
-        <v>74.32162162162162</v>
+        <v>66.26929259530763</v>
       </c>
       <c r="F11" t="n">
-        <v>63.87837837837838</v>
+        <v>84.74013383104247</v>
       </c>
       <c r="G11" t="n">
-        <v>79.76216216216216</v>
+        <v>66.28163934977103</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>Product Designer</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>76.06194690265487</v>
-      </c>
       <c r="C12" t="n">
-        <v>72.74631268436578</v>
+        <v>26.7311540241746</v>
       </c>
       <c r="D12" t="n">
-        <v>59.4424778761062</v>
+        <v>58.33904252544976</v>
       </c>
       <c r="E12" t="n">
-        <v>76.07374631268436</v>
+        <v>118.9597437623324</v>
       </c>
       <c r="F12" t="n">
-        <v>63.6047197640118</v>
+        <v>108.5510808987087</v>
       </c>
       <c r="G12" t="n">
-        <v>80.8613569321534</v>
+        <v>44.66260834377468</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>Project Manager</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>75.75138121546961</v>
-      </c>
       <c r="C13" t="n">
-        <v>70.32044198895028</v>
+        <v>57.81059284620971</v>
       </c>
       <c r="D13" t="n">
-        <v>59.89502762430939</v>
+        <v>28.28673906268114</v>
       </c>
       <c r="E13" t="n">
-        <v>75.39226519337016</v>
+        <v>120.7498675189967</v>
       </c>
       <c r="F13" t="n">
-        <v>64.82320441988951</v>
+        <v>27.79284006792783</v>
       </c>
       <c r="G13" t="n">
-        <v>79.68784530386741</v>
+        <v>47.0029069858396</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>Sales Executive</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v>73.69444444444444</v>
-      </c>
       <c r="C14" t="n">
-        <v>70.125</v>
+        <v>115.7071936317938</v>
       </c>
       <c r="D14" t="n">
-        <v>60.59166666666667</v>
+        <v>67.684081817014</v>
       </c>
       <c r="E14" t="n">
-        <v>74.55277777777778</v>
+        <v>76.24929741873757</v>
       </c>
       <c r="F14" t="n">
-        <v>66.30277777777778</v>
+        <v>73.53801272557061</v>
       </c>
       <c r="G14" t="n">
-        <v>79.61111111111111</v>
+        <v>51.17971753894523</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>Software Engineer</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>75.40322580645162</v>
-      </c>
       <c r="C15" t="n">
-        <v>71.38440860215054</v>
+        <v>90.04919478108739</v>
       </c>
       <c r="D15" t="n">
-        <v>61.87096774193548</v>
+        <v>47.67084159234977</v>
       </c>
       <c r="E15" t="n">
-        <v>74.96505376344086</v>
+        <v>45.79708627600634</v>
       </c>
       <c r="F15" t="n">
-        <v>62.21236559139785</v>
+        <v>29.98705293764506</v>
       </c>
       <c r="G15" t="n">
-        <v>80.3252688172043</v>
+        <v>78.56641314753028</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned up data and added more detaield benchmarking to the dashboard.
</commit_message>
<xml_diff>
--- a/data/Benchmark_Data.xlsx
+++ b/data/Benchmark_Data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,19 +480,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>42.66457320065805</v>
+        <v>67.20473385133047</v>
       </c>
       <c r="D2" t="n">
-        <v>83.44394711474659</v>
+        <v>46.07665320990305</v>
       </c>
       <c r="E2" t="n">
-        <v>110.3736731718898</v>
+        <v>52.85596913433723</v>
       </c>
       <c r="F2" t="n">
-        <v>26.83152524691578</v>
+        <v>42.60660710848016</v>
       </c>
       <c r="G2" t="n">
-        <v>104.8291539435402</v>
+        <v>65.66261747589319</v>
       </c>
     </row>
     <row r="3">
@@ -505,19 +505,19 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>32.07033993460573</v>
+        <v>78.63010069662232</v>
       </c>
       <c r="D3" t="n">
-        <v>51.42882730440155</v>
+        <v>73.33352598562178</v>
       </c>
       <c r="E3" t="n">
-        <v>27.10409715298731</v>
+        <v>41.33022577225088</v>
       </c>
       <c r="F3" t="n">
-        <v>41.3234115956139</v>
+        <v>90.97811146643561</v>
       </c>
       <c r="G3" t="n">
-        <v>81.89001172060458</v>
+        <v>37.94429338693888</v>
       </c>
     </row>
     <row r="4">
@@ -526,23 +526,23 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Customer Support</t>
+          <t>Construction Worker</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>85.90819579932058</v>
+        <v>72.43458032973052</v>
       </c>
       <c r="D4" t="n">
-        <v>91.30494565446023</v>
+        <v>36.39006831610373</v>
       </c>
       <c r="E4" t="n">
-        <v>114.3055978810442</v>
+        <v>43.51467424933426</v>
       </c>
       <c r="F4" t="n">
-        <v>75.29002474858609</v>
+        <v>76.81837814287593</v>
       </c>
       <c r="G4" t="n">
-        <v>91.59631169145987</v>
+        <v>75.45115842914211</v>
       </c>
     </row>
     <row r="5">
@@ -551,23 +551,23 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Data Analyst</t>
+          <t>Customer Support</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>85.24068197080739</v>
+        <v>29.81239756343025</v>
       </c>
       <c r="D5" t="n">
-        <v>53.85237101017578</v>
+        <v>21.56964384126162</v>
       </c>
       <c r="E5" t="n">
-        <v>88.08546543371043</v>
+        <v>53.42496593739565</v>
       </c>
       <c r="F5" t="n">
-        <v>39.26178870883071</v>
+        <v>57.28534498478044</v>
       </c>
       <c r="G5" t="n">
-        <v>57.43328769992886</v>
+        <v>75.75407140709376</v>
       </c>
     </row>
     <row r="6">
@@ -576,23 +576,23 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Data Scientist</t>
+          <t>Data Analyst</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>58.29060015310971</v>
+        <v>112.467889172675</v>
       </c>
       <c r="D6" t="n">
-        <v>24.26173277504419</v>
+        <v>72.9822244490293</v>
       </c>
       <c r="E6" t="n">
-        <v>62.93630877370196</v>
+        <v>37.93595952975845</v>
       </c>
       <c r="F6" t="n">
-        <v>104.9947959832414</v>
+        <v>43.0134711060215</v>
       </c>
       <c r="G6" t="n">
-        <v>80.61764733720652</v>
+        <v>65.08766548335271</v>
       </c>
     </row>
     <row r="7">
@@ -601,23 +601,23 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>HR Specialist</t>
+          <t>Data Scientist</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>98.02336050081948</v>
+        <v>47.97833772166527</v>
       </c>
       <c r="D7" t="n">
-        <v>104.2198591589407</v>
+        <v>94.406976086239</v>
       </c>
       <c r="E7" t="n">
-        <v>47.63064210578121</v>
+        <v>123.8525871669547</v>
       </c>
       <c r="F7" t="n">
-        <v>38.5117707495847</v>
+        <v>53.43798443339365</v>
       </c>
       <c r="G7" t="n">
-        <v>123.9754787741175</v>
+        <v>109.4509584341707</v>
       </c>
     </row>
     <row r="8">
@@ -626,23 +626,23 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Legal Advisor</t>
+          <t>Doctor</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>41.49928456059973</v>
+        <v>115.1250582621385</v>
       </c>
       <c r="D8" t="n">
-        <v>39.41613945827162</v>
+        <v>100.0408759846802</v>
       </c>
       <c r="E8" t="n">
-        <v>117.4910927359335</v>
+        <v>124.1310424330165</v>
       </c>
       <c r="F8" t="n">
-        <v>101.4742991576342</v>
+        <v>16.32924520076737</v>
       </c>
       <c r="G8" t="n">
-        <v>68.95778873870678</v>
+        <v>76.54758765971221</v>
       </c>
     </row>
     <row r="9">
@@ -651,23 +651,23 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Machine Learning Engineer</t>
+          <t>Electrician</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>55.33196789161902</v>
+        <v>80.79870948563672</v>
       </c>
       <c r="D9" t="n">
-        <v>108.0914655182148</v>
+        <v>20.62052569120796</v>
       </c>
       <c r="E9" t="n">
-        <v>121.3040254051418</v>
+        <v>96.23963159904581</v>
       </c>
       <c r="F9" t="n">
-        <v>106.6021677754157</v>
+        <v>102.8259658562364</v>
       </c>
       <c r="G9" t="n">
-        <v>33.11104989979082</v>
+        <v>62.56582209239682</v>
       </c>
     </row>
     <row r="10">
@@ -676,23 +676,23 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Marketing Manager</t>
+          <t>HR Specialist</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>76.93306421135722</v>
+        <v>74.95113270080171</v>
       </c>
       <c r="D10" t="n">
-        <v>11.83680526988351</v>
+        <v>33.76300632014023</v>
       </c>
       <c r="E10" t="n">
-        <v>46.35271529981099</v>
+        <v>65.70514376943694</v>
       </c>
       <c r="F10" t="n">
-        <v>69.34155507426746</v>
+        <v>45.41043831657473</v>
       </c>
       <c r="G10" t="n">
-        <v>59.86941548676152</v>
+        <v>109.0581330574912</v>
       </c>
     </row>
     <row r="11">
@@ -701,23 +701,23 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Operations Manager</t>
+          <t>Legal Advisor</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>117.8684676525102</v>
+        <v>60.77557172992015</v>
       </c>
       <c r="D11" t="n">
-        <v>34.93540751392739</v>
+        <v>99.69559907193678</v>
       </c>
       <c r="E11" t="n">
-        <v>66.26929259530763</v>
+        <v>75.81106431555679</v>
       </c>
       <c r="F11" t="n">
-        <v>84.74013383104247</v>
+        <v>70.98309835611551</v>
       </c>
       <c r="G11" t="n">
-        <v>66.28163934977103</v>
+        <v>50.69110425082442</v>
       </c>
     </row>
     <row r="12">
@@ -726,23 +726,23 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Product Designer</t>
+          <t>Machine Learning Engineer</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>26.7311540241746</v>
+        <v>97.76304832841411</v>
       </c>
       <c r="D12" t="n">
-        <v>58.33904252544976</v>
+        <v>56.57585366599079</v>
       </c>
       <c r="E12" t="n">
-        <v>118.9597437623324</v>
+        <v>25.36446735226679</v>
       </c>
       <c r="F12" t="n">
-        <v>108.5510808987087</v>
+        <v>18.96447130779364</v>
       </c>
       <c r="G12" t="n">
-        <v>44.66260834377468</v>
+        <v>35.09838467933363</v>
       </c>
     </row>
     <row r="13">
@@ -751,23 +751,23 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Project Manager</t>
+          <t>Marketing Manager</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>57.81059284620971</v>
+        <v>109.235535057134</v>
       </c>
       <c r="D13" t="n">
-        <v>28.28673906268114</v>
+        <v>47.13436980365095</v>
       </c>
       <c r="E13" t="n">
-        <v>120.7498675189967</v>
+        <v>106.303752071009</v>
       </c>
       <c r="F13" t="n">
-        <v>27.79284006792783</v>
+        <v>64.65109897466549</v>
       </c>
       <c r="G13" t="n">
-        <v>47.0029069858396</v>
+        <v>127.6185571242596</v>
       </c>
     </row>
     <row r="14">
@@ -776,23 +776,23 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Sales Executive</t>
+          <t>Mechanical Engineer</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>115.7071936317938</v>
+        <v>43.74138976081582</v>
       </c>
       <c r="D14" t="n">
-        <v>67.684081817014</v>
+        <v>79.53369367425483</v>
       </c>
       <c r="E14" t="n">
-        <v>76.24929741873757</v>
+        <v>38.77805462161064</v>
       </c>
       <c r="F14" t="n">
-        <v>73.53801272557061</v>
+        <v>50.67380076399056</v>
       </c>
       <c r="G14" t="n">
-        <v>51.17971753894523</v>
+        <v>72.57105192957494</v>
       </c>
     </row>
     <row r="15">
@@ -801,23 +801,173 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>Nurse</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>37.5766571147183</v>
+      </c>
+      <c r="D15" t="n">
+        <v>34.64945386748243</v>
+      </c>
+      <c r="E15" t="n">
+        <v>32.84387486945073</v>
+      </c>
+      <c r="F15" t="n">
+        <v>110.9899305992184</v>
+      </c>
+      <c r="G15" t="n">
+        <v>84.06646522653472</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Operations Manager</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>30.19232658888301</v>
+      </c>
+      <c r="D16" t="n">
+        <v>23.70128457989871</v>
+      </c>
+      <c r="E16" t="n">
+        <v>72.7759513777151</v>
+      </c>
+      <c r="F16" t="n">
+        <v>39.03099327094822</v>
+      </c>
+      <c r="G16" t="n">
+        <v>80.6410620130309</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Product Designer</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>35.40293979630021</v>
+      </c>
+      <c r="D17" t="n">
+        <v>50.47987470739064</v>
+      </c>
+      <c r="E17" t="n">
+        <v>92.04112859555397</v>
+      </c>
+      <c r="F17" t="n">
+        <v>56.7396242537396</v>
+      </c>
+      <c r="G17" t="n">
+        <v>72.769955636124</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Project Manager</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>108.0975997812136</v>
+      </c>
+      <c r="D18" t="n">
+        <v>32.53923203854022</v>
+      </c>
+      <c r="E18" t="n">
+        <v>53.24497978772666</v>
+      </c>
+      <c r="F18" t="n">
+        <v>80.83670967033808</v>
+      </c>
+      <c r="G18" t="n">
+        <v>74.17440152235834</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Sales Executive</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>96.56955052210475</v>
+      </c>
+      <c r="D19" t="n">
+        <v>106.9302808920604</v>
+      </c>
+      <c r="E19" t="n">
+        <v>97.81915376489032</v>
+      </c>
+      <c r="F19" t="n">
+        <v>65.79838219309795</v>
+      </c>
+      <c r="G19" t="n">
+        <v>67.95297459263324</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>Software Engineer</t>
         </is>
       </c>
-      <c r="C15" t="n">
-        <v>90.04919478108739</v>
-      </c>
-      <c r="D15" t="n">
-        <v>47.67084159234977</v>
-      </c>
-      <c r="E15" t="n">
-        <v>45.79708627600634</v>
-      </c>
-      <c r="F15" t="n">
-        <v>29.98705293764506</v>
-      </c>
-      <c r="G15" t="n">
-        <v>78.56641314753028</v>
+      <c r="C20" t="n">
+        <v>28.54760002264616</v>
+      </c>
+      <c r="D20" t="n">
+        <v>61.7410190091136</v>
+      </c>
+      <c r="E20" t="n">
+        <v>36.23125820436501</v>
+      </c>
+      <c r="F20" t="n">
+        <v>104.2436916048489</v>
+      </c>
+      <c r="G20" t="n">
+        <v>90.15648100482372</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Teacher</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>100.2466061084747</v>
+      </c>
+      <c r="D21" t="n">
+        <v>40.82497456475512</v>
+      </c>
+      <c r="E21" t="n">
+        <v>67.72469838828945</v>
+      </c>
+      <c r="F21" t="n">
+        <v>34.6735428564058</v>
+      </c>
+      <c r="G21" t="n">
+        <v>70.06641566555348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalized PDF and restructure Git Repo
</commit_message>
<xml_diff>
--- a/data/Benchmark_Data.xlsx
+++ b/data/Benchmark_Data.xlsx
@@ -480,19 +480,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>67.20473385133047</v>
+        <v>25.46092070582212</v>
       </c>
       <c r="D2" t="n">
-        <v>46.07665320990305</v>
+        <v>48.89928110391109</v>
       </c>
       <c r="E2" t="n">
-        <v>52.85596913433723</v>
+        <v>29.36823407648259</v>
       </c>
       <c r="F2" t="n">
-        <v>42.60660710848016</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>65.66261747589319</v>
+        <v>79.76887265481093</v>
       </c>
     </row>
     <row r="3">
@@ -505,19 +505,19 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>78.63010069662232</v>
+        <v>35.47070001895196</v>
       </c>
       <c r="D3" t="n">
-        <v>73.33352598562178</v>
+        <v>13.43946833874935</v>
       </c>
       <c r="E3" t="n">
-        <v>41.33022577225088</v>
+        <v>26.33800329683886</v>
       </c>
       <c r="F3" t="n">
-        <v>90.97811146643561</v>
+        <v>44.82603157826325</v>
       </c>
       <c r="G3" t="n">
-        <v>37.94429338693888</v>
+        <v>76.34167738253856</v>
       </c>
     </row>
     <row r="4">
@@ -530,19 +530,19 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>72.43458032973052</v>
+        <v>62.65030358103355</v>
       </c>
       <c r="D4" t="n">
-        <v>36.39006831610373</v>
+        <v>20.328262771856</v>
       </c>
       <c r="E4" t="n">
-        <v>43.51467424933426</v>
+        <v>100</v>
       </c>
       <c r="F4" t="n">
-        <v>76.81837814287593</v>
+        <v>45.0693541582294</v>
       </c>
       <c r="G4" t="n">
-        <v>75.45115842914211</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5">
@@ -555,19 +555,19 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>29.81239756343025</v>
+        <v>53.16831676755705</v>
       </c>
       <c r="D5" t="n">
-        <v>21.56964384126162</v>
+        <v>15.38001080534552</v>
       </c>
       <c r="E5" t="n">
-        <v>53.42496593739565</v>
+        <v>62.04430198085566</v>
       </c>
       <c r="F5" t="n">
-        <v>57.28534498478044</v>
+        <v>43.87679514285356</v>
       </c>
       <c r="G5" t="n">
-        <v>75.75407140709376</v>
+        <v>57.66466763358127</v>
       </c>
     </row>
     <row r="6">
@@ -580,19 +580,19 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>112.467889172675</v>
+        <v>56.72933313736404</v>
       </c>
       <c r="D6" t="n">
-        <v>72.9822244490293</v>
+        <v>80.46100733464016</v>
       </c>
       <c r="E6" t="n">
-        <v>37.93595952975845</v>
+        <v>66.29812480115532</v>
       </c>
       <c r="F6" t="n">
-        <v>43.0134711060215</v>
+        <v>100</v>
       </c>
       <c r="G6" t="n">
-        <v>65.08766548335271</v>
+        <v>29.89297777248765</v>
       </c>
     </row>
     <row r="7">
@@ -605,19 +605,19 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>47.97833772166527</v>
+        <v>79.56627411049811</v>
       </c>
       <c r="D7" t="n">
-        <v>94.406976086239</v>
+        <v>19.48720233820424</v>
       </c>
       <c r="E7" t="n">
-        <v>123.8525871669547</v>
+        <v>94.7708932802425</v>
       </c>
       <c r="F7" t="n">
-        <v>53.43798443339365</v>
+        <v>41.70673899721343</v>
       </c>
       <c r="G7" t="n">
-        <v>109.4509584341707</v>
+        <v>76.58343204936317</v>
       </c>
     </row>
     <row r="8">
@@ -630,19 +630,19 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>115.1250582621385</v>
+        <v>100</v>
       </c>
       <c r="D8" t="n">
-        <v>100.0408759846802</v>
+        <v>14.68810980988851</v>
       </c>
       <c r="E8" t="n">
-        <v>124.1310424330165</v>
+        <v>75.71909102655357</v>
       </c>
       <c r="F8" t="n">
-        <v>16.32924520076737</v>
+        <v>79.27647896967049</v>
       </c>
       <c r="G8" t="n">
-        <v>76.54758765971221</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9">
@@ -655,19 +655,19 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>80.79870948563672</v>
+        <v>61.77368338896039</v>
       </c>
       <c r="D9" t="n">
-        <v>20.62052569120796</v>
+        <v>72.70511039761431</v>
       </c>
       <c r="E9" t="n">
-        <v>96.23963159904581</v>
+        <v>100</v>
       </c>
       <c r="F9" t="n">
-        <v>102.8259658562364</v>
+        <v>76.36980188576024</v>
       </c>
       <c r="G9" t="n">
-        <v>62.56582209239682</v>
+        <v>43.46939083426755</v>
       </c>
     </row>
     <row r="10">
@@ -680,19 +680,19 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>74.95113270080171</v>
+        <v>62.29318466346002</v>
       </c>
       <c r="D10" t="n">
-        <v>33.76300632014023</v>
+        <v>51.51598588623294</v>
       </c>
       <c r="E10" t="n">
-        <v>65.70514376943694</v>
+        <v>90.50399979915296</v>
       </c>
       <c r="F10" t="n">
-        <v>45.41043831657473</v>
+        <v>45.94876242539156</v>
       </c>
       <c r="G10" t="n">
-        <v>109.0581330574912</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11">
@@ -705,19 +705,19 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>60.77557172992015</v>
+        <v>48.36269504309307</v>
       </c>
       <c r="D11" t="n">
-        <v>99.69559907193678</v>
+        <v>24.49163739036445</v>
       </c>
       <c r="E11" t="n">
-        <v>75.81106431555679</v>
+        <v>39.69592121582553</v>
       </c>
       <c r="F11" t="n">
-        <v>70.98309835611551</v>
+        <v>100</v>
       </c>
       <c r="G11" t="n">
-        <v>50.69110425082442</v>
+        <v>73.72837648363699</v>
       </c>
     </row>
     <row r="12">
@@ -730,19 +730,19 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>97.76304832841411</v>
+        <v>26.21767906357819</v>
       </c>
       <c r="D12" t="n">
-        <v>56.57585366599079</v>
+        <v>43.97070949561198</v>
       </c>
       <c r="E12" t="n">
-        <v>25.36446735226679</v>
+        <v>88.21132617235055</v>
       </c>
       <c r="F12" t="n">
-        <v>18.96447130779364</v>
+        <v>83.84160136738717</v>
       </c>
       <c r="G12" t="n">
-        <v>35.09838467933363</v>
+        <v>78.14059510703973</v>
       </c>
     </row>
     <row r="13">
@@ -755,19 +755,19 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>109.235535057134</v>
+        <v>100</v>
       </c>
       <c r="D13" t="n">
-        <v>47.13436980365095</v>
+        <v>76.01442758840712</v>
       </c>
       <c r="E13" t="n">
-        <v>106.303752071009</v>
+        <v>76.24009844570018</v>
       </c>
       <c r="F13" t="n">
-        <v>64.65109897466549</v>
+        <v>37.17206092743768</v>
       </c>
       <c r="G13" t="n">
-        <v>127.6185571242596</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14">
@@ -780,19 +780,19 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>43.74138976081582</v>
+        <v>90.68989183504158</v>
       </c>
       <c r="D14" t="n">
-        <v>79.53369367425483</v>
+        <v>58.30508627637893</v>
       </c>
       <c r="E14" t="n">
-        <v>38.77805462161064</v>
+        <v>100</v>
       </c>
       <c r="F14" t="n">
-        <v>50.67380076399056</v>
+        <v>86.19931411257902</v>
       </c>
       <c r="G14" t="n">
-        <v>72.57105192957494</v>
+        <v>64.38484309842855</v>
       </c>
     </row>
     <row r="15">
@@ -805,19 +805,19 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>37.5766571147183</v>
+        <v>30.81115020868923</v>
       </c>
       <c r="D15" t="n">
-        <v>34.64945386748243</v>
+        <v>48.02463459268451</v>
       </c>
       <c r="E15" t="n">
-        <v>32.84387486945073</v>
+        <v>52.44895385076189</v>
       </c>
       <c r="F15" t="n">
-        <v>110.9899305992184</v>
+        <v>100</v>
       </c>
       <c r="G15" t="n">
-        <v>84.06646522653472</v>
+        <v>95.65773559565649</v>
       </c>
     </row>
     <row r="16">
@@ -830,19 +830,19 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>30.19232658888301</v>
+        <v>55.44047744661044</v>
       </c>
       <c r="D16" t="n">
-        <v>23.70128457989871</v>
+        <v>41.027841706961</v>
       </c>
       <c r="E16" t="n">
-        <v>72.7759513777151</v>
+        <v>100</v>
       </c>
       <c r="F16" t="n">
-        <v>39.03099327094822</v>
+        <v>92.67614514625859</v>
       </c>
       <c r="G16" t="n">
-        <v>80.6410620130309</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17">
@@ -855,19 +855,19 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>35.40293979630021</v>
+        <v>56.56134163456932</v>
       </c>
       <c r="D17" t="n">
-        <v>50.47987470739064</v>
+        <v>30.29428735738359</v>
       </c>
       <c r="E17" t="n">
-        <v>92.04112859555397</v>
+        <v>100</v>
       </c>
       <c r="F17" t="n">
-        <v>56.7396242537396</v>
+        <v>15.46691612318783</v>
       </c>
       <c r="G17" t="n">
-        <v>72.769955636124</v>
+        <v>92.36382799119454</v>
       </c>
     </row>
     <row r="18">
@@ -880,19 +880,19 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>108.0975997812136</v>
+        <v>65.53142484668035</v>
       </c>
       <c r="D18" t="n">
-        <v>32.53923203854022</v>
+        <v>100</v>
       </c>
       <c r="E18" t="n">
-        <v>53.24497978772666</v>
+        <v>100</v>
       </c>
       <c r="F18" t="n">
-        <v>80.83670967033808</v>
+        <v>99.80490147995826</v>
       </c>
       <c r="G18" t="n">
-        <v>74.17440152235834</v>
+        <v>81.5009264733345</v>
       </c>
     </row>
     <row r="19">
@@ -905,19 +905,19 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>96.56955052210475</v>
+        <v>38.10080483931941</v>
       </c>
       <c r="D19" t="n">
-        <v>106.9302808920604</v>
+        <v>8.560731798254054</v>
       </c>
       <c r="E19" t="n">
-        <v>97.81915376489032</v>
+        <v>99.20256804176583</v>
       </c>
       <c r="F19" t="n">
-        <v>65.79838219309795</v>
+        <v>55.34113756524128</v>
       </c>
       <c r="G19" t="n">
-        <v>67.95297459263324</v>
+        <v>40.00522405864503</v>
       </c>
     </row>
     <row r="20">
@@ -930,19 +930,19 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>28.54760002264616</v>
+        <v>28.00689350224013</v>
       </c>
       <c r="D20" t="n">
-        <v>61.7410190091136</v>
+        <v>62.2724052047541</v>
       </c>
       <c r="E20" t="n">
-        <v>36.23125820436501</v>
+        <v>78.96361241406994</v>
       </c>
       <c r="F20" t="n">
-        <v>104.2436916048489</v>
+        <v>100</v>
       </c>
       <c r="G20" t="n">
-        <v>90.15648100482372</v>
+        <v>96.0828309977109</v>
       </c>
     </row>
     <row r="21">
@@ -955,19 +955,19 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>100.2466061084747</v>
+        <v>95.04943788441064</v>
       </c>
       <c r="D21" t="n">
-        <v>40.82497456475512</v>
+        <v>68.77969285782628</v>
       </c>
       <c r="E21" t="n">
-        <v>67.72469838828945</v>
+        <v>30.38223535434911</v>
       </c>
       <c r="F21" t="n">
-        <v>34.6735428564058</v>
+        <v>48.66982999772584</v>
       </c>
       <c r="G21" t="n">
-        <v>70.06641566555348</v>
+        <v>38.51221430445766</v>
       </c>
     </row>
   </sheetData>

</xml_diff>